<commit_message>
News posting test News are readed and posted from excel sheet
</commit_message>
<xml_diff>
--- a/7rMart/src/test/resources/testdata.xlsx
+++ b/7rMart/src/test/resources/testdata.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="News" sheetId="2" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="5">
   <si>
     <t xml:space="preserve">UserName</t>
   </si>
@@ -32,6 +33,9 @@
   </si>
   <si>
     <t xml:space="preserve">invalid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is a news written in excel sheet</t>
   </si>
 </sst>
 </file>
@@ -240,7 +244,7 @@
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -295,4 +299,33 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Replace hardcoded values with data from Excel and Constant class
</commit_message>
<xml_diff>
--- a/7rMart/src/test/resources/testdata.xlsx
+++ b/7rMart/src/test/resources/testdata.xlsx
@@ -5,11 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="1" state="visible" r:id="rId3"/>
     <sheet name="News" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="DeliveryTime" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="Categories" sheetId="4" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
   <si>
     <t xml:space="preserve">UserName</t>
   </si>
@@ -36,14 +38,30 @@
   </si>
   <si>
     <t xml:space="preserve">This is a news written in excel sheet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Food</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electronics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Home Appliances</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beauty</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="hh:mm:ss"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -110,12 +128,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -308,15 +330,93 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="n">
+        <v>0.40625</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C5" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A4"/>
+  <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
code improvement and alingment
</commit_message>
<xml_diff>
--- a/7rMart/src/test/resources/testdata.xlsx
+++ b/7rMart/src/test/resources/testdata.xlsx
@@ -5,13 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="1" state="visible" r:id="rId3"/>
     <sheet name="News" sheetId="2" state="visible" r:id="rId4"/>
     <sheet name="DeliveryTime" sheetId="3" state="visible" r:id="rId5"/>
     <sheet name="Categories" sheetId="4" state="visible" r:id="rId6"/>
+    <sheet name="ConstantValues" sheetId="5" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
   <si>
     <t xml:space="preserve">UserName</t>
   </si>
@@ -53,6 +54,15 @@
   </si>
   <si>
     <t xml:space="preserve">Beauty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Constant Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DELIVERYCHARGELIMIT</t>
   </si>
 </sst>
 </file>
@@ -63,7 +73,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="hh:mm:ss"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -85,6 +95,19 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -128,7 +151,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -138,6 +161,18 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -371,7 +406,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -393,30 +428,73 @@
   </sheetPr>
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="26.57"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="3" t="n">
+        <v>350</v>
       </c>
     </row>
   </sheetData>

</xml_diff>